<commit_message>
Update File for  wireconvert logic
</commit_message>
<xml_diff>
--- a/docs/线束表转化.xlsx
+++ b/docs/线束表转化.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28657B10-2254-4FC8-82B0-DAA9CB203776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E1BBAF-9421-4CB5-89BB-7524C460AAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="线束表转化" sheetId="2" r:id="rId1"/>
@@ -2309,7 +2309,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>热缩管_D9,5/4,8</t>
+    <t>热缩管_Φ19.0/9.5mm_Black</t>
   </si>
 </sst>
 </file>
@@ -2828,6 +2828,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2854,18 +2866,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -5016,8 +5016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6028,11 +6028,11 @@
       <c r="C33" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="66" t="s">
+      <c r="D33" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="67"/>
-      <c r="F33" s="68"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="37">
         <v>1</v>
       </c>
@@ -6054,11 +6054,11 @@
       <c r="C34" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="D34" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="63"/>
       <c r="G34" s="52" t="s">
         <v>534</v>
       </c>
@@ -6074,18 +6074,18 @@
       <c r="A35" s="36">
         <v>2</v>
       </c>
-      <c r="B35" s="15" t="str">
-        <f>VLOOKUP(D35,线束辅料!C17:D21,2,FALSE)</f>
-        <v>DFB00046722</v>
+      <c r="B35" s="15" t="e">
+        <f>VLOOKUP(D35,线束辅料!D17:D21,2,FALSE)</f>
+        <v>#REF!</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="57" t="s">
+      <c r="D35" s="61" t="s">
         <v>539</v>
       </c>
-      <c r="E35" s="58"/>
-      <c r="F35" s="59"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="63"/>
       <c r="G35" s="19">
         <v>0.04</v>
       </c>
@@ -6107,11 +6107,11 @@
       <c r="C36" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="61" t="s">
         <v>297</v>
       </c>
-      <c r="E36" s="58"/>
-      <c r="F36" s="59"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="63"/>
       <c r="G36" s="38">
         <v>1</v>
       </c>
@@ -6127,11 +6127,11 @@
       <c r="A37" s="36"/>
       <c r="B37" s="14"/>
       <c r="C37" s="36"/>
-      <c r="D37" s="60" t="s">
+      <c r="D37" s="64" t="s">
         <v>535</v>
       </c>
-      <c r="E37" s="61"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="17"/>
@@ -6143,9 +6143,9 @@
       <c r="A38" s="36"/>
       <c r="B38" s="14"/>
       <c r="C38" s="36"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="65"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="69"/>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="17"/>
@@ -6163,11 +6163,11 @@
       <c r="C39" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="57" t="s">
+      <c r="D39" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="58"/>
-      <c r="F39" s="59"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="63"/>
       <c r="G39" s="38">
         <v>1</v>
       </c>
@@ -6189,11 +6189,11 @@
       <c r="C40" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="57" t="s">
+      <c r="D40" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="58"/>
-      <c r="F40" s="59"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="63"/>
       <c r="G40" s="20" t="s">
         <v>291</v>
       </c>
@@ -6216,11 +6216,11 @@
       <c r="C41" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="57" t="s">
+      <c r="D41" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="58"/>
-      <c r="F41" s="59"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="63"/>
       <c r="G41" s="38">
         <v>1</v>
       </c>
@@ -6242,11 +6242,11 @@
       <c r="C42" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="57" t="s">
+      <c r="D42" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="58"/>
-      <c r="F42" s="59"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="63"/>
       <c r="G42" s="38">
         <v>1</v>
       </c>
@@ -6262,11 +6262,11 @@
       <c r="A43" s="36"/>
       <c r="B43" s="14"/>
       <c r="C43" s="36"/>
-      <c r="D43" s="60" t="s">
+      <c r="D43" s="64" t="s">
         <v>536</v>
       </c>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="17"/>
@@ -6278,9 +6278,9 @@
       <c r="A44" s="36"/>
       <c r="B44" s="14"/>
       <c r="C44" s="36"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
       <c r="G44" s="21"/>
       <c r="H44" s="21"/>
       <c r="I44" s="17"/>
@@ -6298,11 +6298,11 @@
       <c r="C45" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="57" t="s">
+      <c r="D45" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="58"/>
-      <c r="F45" s="59"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="63"/>
       <c r="G45" s="19">
         <v>0.04</v>
       </c>
@@ -6324,11 +6324,11 @@
       <c r="C46" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="57" t="s">
+      <c r="D46" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="E46" s="58"/>
-      <c r="F46" s="59"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="63"/>
       <c r="G46" s="52">
         <v>3</v>
       </c>
@@ -6426,11 +6426,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D39:F39"/>
     <mergeCell ref="D45:F45"/>
     <mergeCell ref="D46:F46"/>
     <mergeCell ref="D37:F38"/>
@@ -6438,6 +6433,11 @@
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D42:F42"/>
     <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D39:F39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F4:F6">
@@ -6633,7 +6633,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{51871BBE-8C39-4CB3-966E-99478194D0A3}">
           <x14:formula1>
-            <xm:f>线束辅料!$C$17:$C$21</xm:f>
+            <xm:f>线束辅料!$D$17:$D$21</xm:f>
           </x14:formula1>
           <xm:sqref>D35:F35</xm:sqref>
         </x14:dataValidation>
@@ -6648,14 +6648,14 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="22.75" customWidth="1"/>
-    <col min="3" max="3" width="53.25" customWidth="1"/>
-    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="4" max="4" width="53.25" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6673,10 +6673,10 @@
         <v>298</v>
       </c>
       <c r="C2" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="45" t="s">
         <v>296</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>295</v>
       </c>
       <c r="E2" s="45" t="s">
         <v>305</v>
@@ -6689,11 +6689,11 @@
       <c r="B3" s="41">
         <v>16</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>79</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>78</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>43</v>
@@ -6706,11 +6706,11 @@
       <c r="B4" s="25">
         <v>16</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>82</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>43</v>
@@ -6726,11 +6726,11 @@
       <c r="B5" s="25">
         <v>25</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>85</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>84</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>43</v>
@@ -6746,11 +6746,11 @@
       <c r="B6" s="25">
         <v>50</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>87</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>86</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>43</v>
@@ -6763,11 +6763,11 @@
       <c r="B7" s="25">
         <v>50</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>88</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>43</v>
@@ -6783,11 +6783,11 @@
       <c r="B8" s="47" t="s">
         <v>319</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="49" t="s">
         <v>91</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>90</v>
       </c>
       <c r="E8" s="49" t="s">
         <v>43</v>
@@ -6806,11 +6806,11 @@
       <c r="B9" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="49" t="s">
         <v>94</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>93</v>
       </c>
       <c r="E9" s="49" t="s">
         <v>43</v>
@@ -6826,11 +6826,11 @@
       <c r="B10" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>97</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>96</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>43</v>
@@ -6846,11 +6846,11 @@
       <c r="B11" s="25">
         <v>0.34</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="E11" s="26" t="s">
         <v>306</v>
@@ -6863,11 +6863,11 @@
       <c r="B12" s="25">
         <v>0.5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>43</v>
@@ -6880,11 +6880,11 @@
       <c r="B13" s="25">
         <v>1</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="15">
+        <v>12024613</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>73</v>
-      </c>
-      <c r="D13" s="15">
-        <v>12024613</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>43</v>
@@ -6897,11 +6897,11 @@
       <c r="B14" s="25">
         <v>1.5</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>74</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>43</v>
@@ -6917,11 +6917,11 @@
       <c r="B15" s="25">
         <v>2.5</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>77</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>76</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>43</v>
@@ -6934,11 +6934,11 @@
       <c r="B16" s="25">
         <v>16</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>80</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>43</v>
@@ -6952,11 +6952,11 @@
       <c r="B17" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>101</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>311</v>
@@ -6978,11 +6978,11 @@
       <c r="B18" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="E18" s="26" t="s">
         <v>311</v>
@@ -6995,11 +6995,11 @@
       <c r="B19" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>106</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>311</v>
@@ -7012,11 +7012,11 @@
       <c r="B20" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>110</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>311</v>
@@ -7029,11 +7029,11 @@
       <c r="B21" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>113</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>112</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>311</v>
@@ -7046,11 +7046,11 @@
       <c r="B22" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>120</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>43</v>
@@ -7072,11 +7072,11 @@
       <c r="B23" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>124</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>43</v>
@@ -7092,11 +7092,11 @@
       <c r="B24" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>126</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>43</v>
@@ -7109,10 +7109,10 @@
       <c r="B25" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="54"/>
+      <c r="D25" s="49" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="54"/>
       <c r="E25" s="26" t="s">
         <v>327</v>
       </c>
@@ -7124,11 +7124,11 @@
       <c r="B26" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="26" t="s">
         <v>116</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>43</v>
@@ -7144,11 +7144,11 @@
       <c r="B27" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>515</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>118</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>43</v>
@@ -7168,8 +7168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487186A3-9D00-4197-A303-5F818918C0BB}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7625,7 +7625,7 @@
       <c r="E20" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="F20" s="69" t="s">
+      <c r="F20" s="57" t="s">
         <v>538</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -7648,7 +7648,7 @@
       <c r="E21" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="F21" s="69" t="s">
+      <c r="F21" s="57" t="s">
         <v>538</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -7740,7 +7740,7 @@
       <c r="E25" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="F25" s="69" t="s">
+      <c r="F25" s="57" t="s">
         <v>538</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -8346,7 +8346,7 @@
       <c r="E51" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="F51" s="69" t="s">
+      <c r="F51" s="57" t="s">
         <v>538</v>
       </c>
       <c r="G51" s="2" t="s">

</xml_diff>